<commit_message>
Score Matrix is added
</commit_message>
<xml_diff>
--- a/MainDatabase/Real.xlsx
+++ b/MainDatabase/Real.xlsx
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,16 +1030,16 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12602</v>
+        <v>11420</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1048,13 +1048,13 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1063,10 +1063,10 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M15">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>9138</v>
+        <v>12602</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1086,16 +1086,16 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H16">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1104,13 +1104,13 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="M16">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11366</v>
+        <v>8693</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1139,22 +1139,22 @@
         <v>6</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M17">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>11389</v>
+        <v>9138</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1171,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1189,16 +1189,16 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L18">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="M18">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -1206,16 +1206,16 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>8895</v>
+        <v>11366</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1233,16 +1233,16 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K19">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M19">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8874</v>
+        <v>11389</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1268,25 +1268,25 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>19</v>
       </c>
       <c r="M20">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -1294,10 +1294,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>11368</v>
+        <v>8895</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1309,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1321,16 +1321,16 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L21">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="M21">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -1338,19 +1338,19 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>8693</v>
+        <v>8874</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1359,7 +1359,7 @@
         <v>6</v>
       </c>
       <c r="H22">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1368,13 +1368,13 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M22">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>9395</v>
+        <v>11368</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1394,28 +1394,28 @@
         <v>3</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K23">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="M23">
         <v>29</v>
@@ -1426,13 +1426,13 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>9110</v>
+        <v>8693</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>4</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>6</v>
@@ -1450,27 +1450,27 @@
         <v>7</v>
       </c>
       <c r="I24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="M24">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9703</v>
+        <v>9395</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1485,13 +1485,13 @@
         <v>4</v>
       </c>
       <c r="F25">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I25">
         <v>8</v>
@@ -1503,18 +1503,18 @@
         <v>10</v>
       </c>
       <c r="L25">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="M25">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="N25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>8229</v>
+        <v>9110</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1523,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -1532,25 +1532,25 @@
         <v>5</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H26">
         <v>7</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K26">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L26">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="M26">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1558,22 +1558,22 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>12595</v>
+        <v>9703</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <v>4</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1585,16 +1585,16 @@
         <v>8</v>
       </c>
       <c r="J27">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L27">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="M27">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1602,31 +1602,31 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>11412</v>
+        <v>8229</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <v>4</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I28">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -1635,10 +1635,10 @@
         <v>10</v>
       </c>
       <c r="L28">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="M28">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -1646,19 +1646,19 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>11130</v>
+        <v>12595</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1670,16 +1670,16 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J29">
         <v>9</v>
       </c>
       <c r="K29">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L29">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M29">
         <v>40</v>
@@ -1690,25 +1690,25 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>11410</v>
+        <v>11412</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1720,19 +1720,108 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L30">
+        <v>22</v>
+      </c>
+      <c r="M30">
+        <v>40</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>11130</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>9</v>
+      </c>
+      <c r="K31">
+        <v>10</v>
+      </c>
+      <c r="L31">
+        <v>25</v>
+      </c>
+      <c r="M31">
+        <v>40</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11410</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>6</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
         <v>19</v>
       </c>
-      <c r="M30">
+      <c r="M32">
         <v>37</v>
       </c>
-      <c r="N30">
+      <c r="N32">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>